<commit_message>
added new test : Manish
</commit_message>
<xml_diff>
--- a/src/main/java/TestData/TestData.xlsx
+++ b/src/main/java/TestData/TestData.xlsx
@@ -1,75 +1,220 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\FrontendAutomation\src\main\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\CA_Automation\src\main\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F6961D-CE70-4EF9-A091-E2D0EE06C4B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8836EC-8645-45DB-AE44-55DEA1B2B88B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="Deals" sheetId="4" r:id="rId2"/>
-    <sheet name="Tasks" sheetId="5" r:id="rId3"/>
+    <sheet name="AmazonTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Mr.</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>Dr.</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Cris</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>Mrs.</t>
-  </si>
-  <si>
-    <t>Ebay</t>
-  </si>
-  <si>
-    <t>Muktha</t>
-  </si>
-  <si>
-    <t>Sharma</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+  <si>
+    <t>sl no</t>
+  </si>
+  <si>
+    <t>test Case ID</t>
+  </si>
+  <si>
+    <t>Test Category</t>
+  </si>
+  <si>
+    <t>Need to Run?</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Sanity</t>
+  </si>
+  <si>
+    <t>validateURLNavigation</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Verify webpage is redirected to correct url</t>
+  </si>
+  <si>
+    <t>1. launch amazon site.
+2. verify redirected url</t>
+  </si>
+  <si>
+    <t>Online Shopping site in India: Shop Online for Mobiles, Books, Watches, Shoes and More - Amazon.in</t>
+  </si>
+  <si>
+    <t>validateTitleNavigation</t>
+  </si>
+  <si>
+    <t>validateCreateWishListNavigation</t>
+  </si>
+  <si>
+    <t>validateSearchResult</t>
+  </si>
+  <si>
+    <t>validateDeliveryPinSelected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify title of webpage displayed correctly </t>
+  </si>
+  <si>
+    <t>Verify user is able navigate to wishlist page</t>
+  </si>
+  <si>
+    <t>Verify user is able to perform search</t>
+  </si>
+  <si>
+    <t>1. launch amazon site.
+2. verify title of website is correct</t>
+  </si>
+  <si>
+    <t>1. launch amazon site.
+2. click on wishlist link
+3. verify title of page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. launch amazon site.
+2. click on search text box 
+3. enter serach text
+4. verify search result displayed </t>
+  </si>
+  <si>
+    <t>validateUserIsAbleToSelectfourStarRating</t>
+  </si>
+  <si>
+    <t>validateUserIsAbleToClickOnFristProduct</t>
+  </si>
+  <si>
+    <t>validateDealPriceDisplayed</t>
+  </si>
+  <si>
+    <t>validateMRPDisplayed</t>
+  </si>
+  <si>
+    <t>validateDeliveryDateDisplayed</t>
+  </si>
+  <si>
+    <t>testData-amazon</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Amazon.in: mi mobile - 4 Stars &amp; Up</t>
+  </si>
+  <si>
+    <t>mi mobile</t>
+  </si>
+  <si>
+    <t>Amazon.in</t>
+  </si>
+  <si>
+    <t>412101</t>
+  </si>
+  <si>
+    <t>1. launch amazon site.
+2. perform search
+3. very user is able to filter product with 4 star rating</t>
+  </si>
+  <si>
+    <t>1. launch amazon site.
+2. perform search
+3. verify user is able to open frist product</t>
+  </si>
+  <si>
+    <t>1. launch amazon site.
+2. perform search
+3. click on frist product
+4. verify deal price displayed</t>
+  </si>
+  <si>
+    <t>1. launch amazon site.
+2. perform search
+3. click on frist product
+4. verify MRP displayed</t>
+  </si>
+  <si>
+    <t>1. launch amazon site.
+2. perform search
+3. click on frist product
+4. verify delivery delivery date displayed</t>
+  </si>
+  <si>
+    <t>1. launch amazon site.
+2. perform search
+3. click on frist product
+4. enter location pin
+4. verify delivery location displayed</t>
+  </si>
+  <si>
+    <t>expected result</t>
+  </si>
+  <si>
+    <t>website is redirected to amazon.in</t>
+  </si>
+  <si>
+    <t>title should be displayed correctly</t>
+  </si>
+  <si>
+    <t>title of wishlist page should be displayed correctly</t>
+  </si>
+  <si>
+    <t>user should be able to search product</t>
+  </si>
+  <si>
+    <t>user should be able filter product with 4 start rating</t>
+  </si>
+  <si>
+    <t>user should be able open frist product</t>
+  </si>
+  <si>
+    <t>Verify user is able to filter with 4 star product</t>
+  </si>
+  <si>
+    <t>Verify user is able to open frist product</t>
+  </si>
+  <si>
+    <t>Verify deal price displayed correctly</t>
+  </si>
+  <si>
+    <t>Verify MRP displayed correctly</t>
+  </si>
+  <si>
+    <t>Verify Delivery date displayed correctly</t>
+  </si>
+  <si>
+    <t>Verify user is able to select location</t>
+  </si>
+  <si>
+    <t>user should be able to select location</t>
+  </si>
+  <si>
+    <t>Delivery date should be displayed correctly</t>
+  </si>
+  <si>
+    <t>MRP should be displayed correclty</t>
+  </si>
+  <si>
+    <t>Deal price should be displayed correclty</t>
+  </si>
+  <si>
+    <t>Redmi</t>
   </si>
 </sst>
 </file>
@@ -85,21 +230,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -108,15 +247,108 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -126,13 +358,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,101 +715,318 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.7265625" customWidth="1"/>
+    <col min="6" max="7" width="46.453125" customWidth="1"/>
+    <col min="8" max="8" width="47.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
+      <c r="B8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D11" xr:uid="{A3E196F4-A8AB-4525-8F50-4196A13B3684}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C11" xr:uid="{F9838CF0-68B8-4ACF-AC5E-5F80E8C49FAD}">
+      <formula1>"Sanity,Regression,Functional"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>